<commit_message>
Update Dataset, Add classify function
데이터셋 추가, 분류 라벨에 따른 결과값 저장함수 추가
</commit_message>
<xml_diff>
--- a/Evaluation Table.xlsx
+++ b/Evaluation Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jim51\OneDrive\바탕 화면\레포\Predicting-RBP-binding-with-CNN-Capsnet-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jim51\OneDrive\바탕화~1\레포\PREDIC~1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E4F0A0-B39C-4578-87E4-771D15F23EF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0B96EB-6B3A-46EA-AE76-0954D7AB9D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33870" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{2369E03F-A5CA-4C2C-945B-0572066FCC40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2369E03F-A5CA-4C2C-945B-0572066FCC40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -113,6 +113,46 @@
   </si>
   <si>
     <t>CNN_base_model_k_fold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>new Pyfeat Data 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train: test = 7:3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train: test = 7:3 -kfold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train: test = 8:2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train: test = 8:2 -kfold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train: test = 5:5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정확도 66 ~72사이에서 변동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train: test = 5:5 -kfold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이어 설정 base_model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -477,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F40CC1B-6460-4BEC-AB76-D2E6B08A8D90}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -489,7 +529,7 @@
     <col min="2" max="8" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -540,8 +580,11 @@
       <c r="H2">
         <v>0.499</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -567,7 +610,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -593,7 +636,7 @@
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -619,7 +662,7 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -645,7 +688,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -671,7 +714,7 @@
         <v>0.93500000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -697,7 +740,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -723,7 +766,7 @@
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -749,7 +792,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -775,7 +818,7 @@
         <v>0.82299999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -801,7 +844,7 @@
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -825,6 +868,212 @@
       </c>
       <c r="H13">
         <v>0.97199999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="C17">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="D17">
+        <v>0.5333</v>
+      </c>
+      <c r="E17">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="F17">
+        <v>0.72</v>
+      </c>
+      <c r="G17">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="L17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="C18">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D18">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="E18">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F18">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="G18">
+        <v>0.94</v>
+      </c>
+      <c r="H18">
+        <v>0.98</v>
+      </c>
+      <c r="L18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="C19">
+        <v>0.88</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="F19">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G19">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="H19">
+        <v>0.745</v>
+      </c>
+      <c r="L19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="C20">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="C21">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="D21">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="E21">
+        <v>0.67</v>
+      </c>
+      <c r="F21">
+        <v>0.88</v>
+      </c>
+      <c r="G21">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="H21">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="C22">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="D22">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="E22">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="F22">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="G22">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="H22">
+        <v>0.997</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>